<commit_message>
added the updated info
</commit_message>
<xml_diff>
--- a/database/Additional Info/IndexToTable.xlsx
+++ b/database/Additional Info/IndexToTable.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\apers\OneDrive\Desktop\484 Files\lab1_P3\Additional Info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B0421FD-8894-4E9E-82AD-9B06AB3BAB06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE7C7415-E8F0-4205-9086-41C1ADB18084}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4D608147-E7B5-4818-8A35-A1AAA5944482}"/>
   </bookViews>
@@ -527,7 +527,7 @@
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:C5"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>